<commit_message>
Auto update all files
</commit_message>
<xml_diff>
--- a/data/raw/cz_drill.xlsx
+++ b/data/raw/cz_drill.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files x86\A Study File\mycode\LSTM\CZstandard\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D553F753-B96E-4F15-8A99-F02C57E1C6F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7856D57-FE2C-4667-A8D8-B38ADB2F6D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -392,7 +392,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -402,6 +402,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -433,7 +445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -452,6 +464,13 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -735,7 +754,7 @@
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -744,13 +763,14 @@
     <col min="2" max="2" width="20.1640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.4140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="11.25" style="2" customWidth="1"/>
-    <col min="5" max="9" width="12.58203125" style="2" customWidth="1"/>
+    <col min="5" max="8" width="12.58203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12.58203125" style="10" customWidth="1"/>
     <col min="10" max="10" width="15" style="2" customWidth="1"/>
     <col min="11" max="11" width="15.1640625" style="2" customWidth="1"/>
     <col min="12" max="12" width="14.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="95.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="72.5" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="4" t="s">
         <v>3</v>
@@ -773,7 +793,7 @@
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="9" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="6" t="s">
@@ -787,344 +807,344 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="8">
         <v>3</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="8">
         <v>4.92</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="8">
         <v>2.74</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="8">
         <v>16.2</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="8">
         <v>0.23</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="8">
         <v>6.87</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="8">
         <v>2.2000000000000002</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="9">
         <v>1.59</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="8">
         <v>2.73</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="8">
         <v>187.87</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="8">
         <v>190.6</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
+      <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="8">
         <v>3</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="8">
         <v>7.21</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="8">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="8">
         <v>26.04</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="8">
         <v>0.2</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="8">
         <v>5.87</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="8">
         <v>1.93</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="9">
         <v>1.56</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="8">
         <v>2.4</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="8">
         <v>191.45</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="8">
         <v>193.85</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+      <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="8">
         <v>3</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="8">
         <v>4.2699999999999996</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="8">
         <v>7.21</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="8">
         <v>45.28</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="8">
         <v>0.19</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="8">
         <v>4.4400000000000004</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="8">
         <v>1.83</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="9">
         <v>1.25</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="8">
         <v>2.27</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="8">
         <v>475.35</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="8">
         <v>478.24</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+      <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="8">
         <v>3</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="8">
         <v>36</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="8">
         <v>2.37</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="8">
         <v>17.170000000000002</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="8">
         <v>0.19</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="8">
         <v>14.9</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="8">
         <v>1.79</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="9">
         <v>1.35</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="8">
         <v>2.5499999999999998</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="8">
         <v>85.08</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="8">
         <v>87.63</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+      <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="8">
         <v>3</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="8">
         <v>33.67</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="8">
         <v>4.32</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="8">
         <v>27.74</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="8">
         <v>0.22</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="8">
         <v>13.11</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="8">
         <v>2.04</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="9">
         <v>1.3</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="8">
         <v>2.23</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="8">
         <v>55.51</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="8">
         <v>57.74</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+      <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="8">
         <v>3</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="8">
         <v>37.450000000000003</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="8">
         <v>7.33</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="8">
         <v>46.13</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="8">
         <v>0.19</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="8">
         <v>9.48</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="8">
         <v>1.82</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="9">
         <v>1.4</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="8">
         <v>2.2599999999999998</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="8">
         <v>92.28</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="8">
         <v>94.53</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
+      <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="8">
         <v>3</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="8">
         <v>52</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="8">
         <v>2.71</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="8">
         <v>17.329999999999998</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="8">
         <v>0.31</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="8">
         <v>27.18</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="8">
         <v>2.94</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="9">
         <v>1.34</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="8">
         <v>3.66</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="8">
         <v>70.930000000000007</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8" s="8">
         <v>74.59</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
+      <c r="A9" s="8">
         <v>8</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="8">
         <v>3</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="8">
         <v>59.33</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="8">
         <v>3.66</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="8">
         <v>23.03</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="8">
         <v>0.26</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="8">
         <v>21.58</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="8">
         <v>2.44</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="9">
         <v>1.33</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="8">
         <v>3.38</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="8">
         <v>64.69</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9" s="8">
         <v>68.069999999999993</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
+      <c r="A10" s="8">
         <v>9</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="8">
         <v>3</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="8">
         <v>61.5</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="8">
         <v>6.75</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="8">
         <v>42.39</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="8">
         <v>0.2</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="8">
         <v>13.72</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="8">
         <v>1.89</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="9">
         <v>1.28</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="8">
         <v>2.35</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="8">
         <v>74.28</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10" s="8">
         <v>76.64</v>
       </c>
     </row>
@@ -1153,7 +1173,7 @@
       <c r="H11" s="4">
         <v>2.0299999999999998</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="9">
         <v>1.24</v>
       </c>
       <c r="J11" s="4">
@@ -1191,7 +1211,7 @@
       <c r="H12" s="4">
         <v>1.63</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="9">
         <v>1.08</v>
       </c>
       <c r="J12" s="4">
@@ -1229,7 +1249,7 @@
       <c r="H13" s="4">
         <v>1.62</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="9">
         <v>1.06</v>
       </c>
       <c r="J13" s="4">
@@ -1267,7 +1287,7 @@
       <c r="H14" s="4">
         <v>2.69</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="9">
         <v>1.03</v>
       </c>
       <c r="J14" s="4">
@@ -1305,7 +1325,7 @@
       <c r="H15" s="4">
         <v>2.33</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="9">
         <v>1.05</v>
       </c>
       <c r="J15" s="4">
@@ -1343,7 +1363,7 @@
       <c r="H16" s="4">
         <v>1.99</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I16" s="9">
         <v>0.93</v>
       </c>
       <c r="J16" s="4">
@@ -1381,7 +1401,7 @@
       <c r="H17" s="4">
         <v>3.64</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="9">
         <v>0.99</v>
       </c>
       <c r="J17" s="4">
@@ -1419,7 +1439,7 @@
       <c r="H18" s="4">
         <v>2.78</v>
       </c>
-      <c r="I18" s="4">
+      <c r="I18" s="9">
         <v>1.07</v>
       </c>
       <c r="J18" s="4">
@@ -1457,7 +1477,7 @@
       <c r="H19" s="4">
         <v>2.36</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I19" s="9">
         <v>1.05</v>
       </c>
       <c r="J19" s="4">
@@ -1471,344 +1491,344 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="4">
+      <c r="A20" s="8">
         <v>1</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="8">
         <v>6.7</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="8">
         <v>10.119999999999999</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="8">
         <v>2.5099999999999998</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="8">
         <v>15.79</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="8">
         <v>0.22</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="8">
         <v>15.38</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="8">
         <v>2.09</v>
       </c>
-      <c r="I20" s="4">
+      <c r="I20" s="9">
         <v>0.9</v>
       </c>
-      <c r="J20" s="4">
+      <c r="J20" s="8">
         <v>2.6</v>
       </c>
-      <c r="K20" s="4">
+      <c r="K20" s="8">
         <v>195.57</v>
       </c>
-      <c r="L20" s="4">
+      <c r="L20" s="8">
         <v>198.17</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4">
+      <c r="A21" s="8">
         <v>2</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="8">
         <v>6.7</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="8">
         <v>9.85</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="8">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="8">
         <v>25.71</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="8">
         <v>0.21</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="8">
         <v>11.79</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21" s="8">
         <v>1.99</v>
       </c>
-      <c r="I21" s="4">
+      <c r="I21" s="9">
         <v>0.91</v>
       </c>
-      <c r="J21" s="4">
+      <c r="J21" s="8">
         <v>2.48</v>
       </c>
-      <c r="K21" s="4">
+      <c r="K21" s="8">
         <v>266.04899999999998</v>
       </c>
-      <c r="L21" s="4">
+      <c r="L21" s="8">
         <v>268.52</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="4">
+      <c r="A22" s="8">
         <v>3</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="8">
         <v>6.7</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="8">
         <v>9.92</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="8">
         <v>6.49</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="8">
         <v>40.909999999999997</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="8">
         <v>0.2</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="8">
         <v>9.75</v>
       </c>
-      <c r="H22" s="4">
+      <c r="H22" s="8">
         <v>1.88</v>
       </c>
-      <c r="I22" s="4">
+      <c r="I22" s="9">
         <v>0.87</v>
       </c>
-      <c r="J22" s="4">
+      <c r="J22" s="8">
         <v>2.34</v>
       </c>
-      <c r="K22" s="4">
+      <c r="K22" s="8">
         <v>338.29</v>
       </c>
-      <c r="L22" s="4">
+      <c r="L22" s="8">
         <v>340.62</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="4">
+      <c r="A23" s="8">
         <v>4</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="8">
         <v>6.7</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="8">
         <v>24.5</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="8">
         <v>2.59</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="8">
         <v>16.22</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="8">
         <v>0.31</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="8">
         <v>33.159999999999997</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H23" s="8">
         <v>2.98</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I23" s="9">
         <v>0.86</v>
       </c>
-      <c r="J23" s="4">
+      <c r="J23" s="8">
         <v>3.7</v>
       </c>
-      <c r="K23" s="4">
+      <c r="K23" s="8">
         <v>172.6</v>
       </c>
-      <c r="L23" s="4">
+      <c r="L23" s="8">
         <v>176.3</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="4">
+      <c r="A24" s="8">
         <v>5</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="8">
         <v>6.7</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="8">
         <v>29.45</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="8">
         <v>4.18</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="8">
         <v>26.15</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F24" s="8">
         <v>0.24</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="8">
         <v>23</v>
       </c>
-      <c r="H24" s="4">
+      <c r="H24" s="8">
         <v>2.3199999999999998</v>
       </c>
-      <c r="I24" s="4">
+      <c r="I24" s="9">
         <v>0.85</v>
       </c>
-      <c r="J24" s="4">
+      <c r="J24" s="8">
         <v>2.92</v>
       </c>
-      <c r="K24" s="4">
+      <c r="K24" s="8">
         <v>159.68</v>
       </c>
-      <c r="L24" s="4">
+      <c r="L24" s="8">
         <v>162.6</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="4">
+      <c r="A25" s="8">
         <v>6</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="8">
         <v>6.7</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="8">
         <v>26.15</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="8">
         <v>5.29</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="8">
         <v>33.22</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F25" s="8">
         <v>0.27</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="8">
         <v>21.56</v>
       </c>
-      <c r="H25" s="4">
+      <c r="H25" s="8">
         <v>2.5499999999999998</v>
       </c>
-      <c r="I25" s="4">
+      <c r="I25" s="9">
         <v>0.86</v>
       </c>
-      <c r="J25" s="4">
+      <c r="J25" s="8">
         <v>3.17</v>
       </c>
-      <c r="K25" s="4">
+      <c r="K25" s="8">
         <v>214.11</v>
       </c>
-      <c r="L25" s="4">
+      <c r="L25" s="8">
         <v>217.28</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="4">
+      <c r="A26" s="8">
         <v>7</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="8">
         <v>6.7</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="8">
         <v>33</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D26" s="8">
         <v>2.59</v>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="8">
         <v>16.170000000000002</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F26" s="8">
         <v>0.43</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G26" s="8">
         <v>48.06</v>
       </c>
-      <c r="H26" s="4">
+      <c r="H26" s="8">
         <v>4.07</v>
       </c>
-      <c r="I26" s="4">
+      <c r="I26" s="9">
         <v>0.91</v>
       </c>
-      <c r="J26" s="4">
+      <c r="J26" s="8">
         <v>5.0599999999999996</v>
       </c>
-      <c r="K26" s="4">
+      <c r="K26" s="8">
         <v>185.33</v>
       </c>
-      <c r="L26" s="4">
+      <c r="L26" s="8">
         <v>190.3</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="4">
+      <c r="A27" s="8">
         <v>8</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="8">
         <v>6.7</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="8">
         <v>49.67</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D27" s="8">
         <v>4.5599999999999996</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="8">
         <v>28.68</v>
       </c>
-      <c r="F27" s="4">
+      <c r="F27" s="8">
         <v>0.36</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27" s="8">
         <v>37.5</v>
       </c>
-      <c r="H27" s="4">
+      <c r="H27" s="8">
         <v>3.41</v>
       </c>
-      <c r="I27" s="4">
+      <c r="I27" s="9">
         <v>0.91</v>
       </c>
-      <c r="J27" s="4">
+      <c r="J27" s="8">
         <v>4.24</v>
       </c>
-      <c r="K27" s="4">
+      <c r="K27" s="8">
         <v>168.81</v>
       </c>
-      <c r="L27" s="4">
+      <c r="L27" s="8">
         <v>173.05</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="4">
+      <c r="A28" s="8">
         <v>9</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="8">
         <v>6.7</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="8">
         <v>51.2</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="8">
         <v>5.72</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="8">
         <v>35.92</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F28" s="8">
         <v>0.34</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="8">
         <v>43.6</v>
       </c>
-      <c r="H28" s="4">
+      <c r="H28" s="8">
         <v>3.22</v>
       </c>
-      <c r="I28" s="4">
+      <c r="I28" s="9">
         <v>0.86</v>
       </c>
-      <c r="J28" s="4">
+      <c r="J28" s="8">
         <v>4</v>
       </c>
-      <c r="K28" s="4">
+      <c r="K28" s="8">
         <v>189.95</v>
       </c>
-      <c r="L28" s="4">
+      <c r="L28" s="8">
         <v>193.95</v>
       </c>
     </row>
@@ -1837,7 +1857,7 @@
       <c r="H29" s="4">
         <v>2.1</v>
       </c>
-      <c r="I29" s="4">
+      <c r="I29" s="9">
         <v>0.69</v>
       </c>
       <c r="J29" s="4">
@@ -1875,7 +1895,7 @@
       <c r="H30" s="4">
         <v>1.76</v>
       </c>
-      <c r="I30" s="4">
+      <c r="I30" s="9">
         <v>0.64</v>
       </c>
       <c r="J30" s="4">
@@ -1913,7 +1933,7 @@
       <c r="H31" s="4">
         <v>1.71</v>
       </c>
-      <c r="I31" s="4">
+      <c r="I31" s="9">
         <v>0.65</v>
       </c>
       <c r="J31" s="4">
@@ -1951,7 +1971,7 @@
       <c r="H32" s="4">
         <v>2.67</v>
       </c>
-      <c r="I32" s="4">
+      <c r="I32" s="9">
         <v>0.66</v>
       </c>
       <c r="J32" s="4">
@@ -1989,7 +2009,7 @@
       <c r="H33" s="4">
         <v>2.5299999999999998</v>
       </c>
-      <c r="I33" s="4">
+      <c r="I33" s="9">
         <v>0.71</v>
       </c>
       <c r="J33" s="4">
@@ -2027,7 +2047,7 @@
       <c r="H34" s="4">
         <v>1.97</v>
       </c>
-      <c r="I34" s="4">
+      <c r="I34" s="9">
         <v>0.66</v>
       </c>
       <c r="J34" s="4">
@@ -2065,7 +2085,7 @@
       <c r="H35" s="4">
         <v>2.8</v>
       </c>
-      <c r="I35" s="4">
+      <c r="I35" s="9">
         <v>0.62</v>
       </c>
       <c r="J35" s="4">
@@ -2103,7 +2123,7 @@
       <c r="H36" s="4">
         <v>3.03</v>
       </c>
-      <c r="I36" s="4">
+      <c r="I36" s="9">
         <v>0.72</v>
       </c>
       <c r="J36" s="4">
@@ -2141,7 +2161,7 @@
       <c r="H37" s="4">
         <v>2.73</v>
       </c>
-      <c r="I37" s="4">
+      <c r="I37" s="9">
         <v>0.7</v>
       </c>
       <c r="J37" s="4">

</xml_diff>